<commit_message>
modified job posting dict
</commit_message>
<xml_diff>
--- a/code/team69.xlsx
+++ b/code/team69.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChristineKu\Desktop\Cornell Tech\Fall 2019\Product Studio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChristineKu\Documents\GitHub\F19-T069\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BDCB189-281C-4522-AB95-83DA9B93C076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FB8AA7-B004-4B01-A965-6EE0D86AEE1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="1220" windowWidth="14400" windowHeight="7360" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Refugee Profile Inputs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="131">
   <si>
     <t>Manual - Jobs</t>
   </si>
@@ -403,6 +403,21 @@
   </si>
   <si>
     <t>Taking care of infants (under 1yo), cooking, attentive</t>
+  </si>
+  <si>
+    <t>Technical</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Professional</t>
+  </si>
+  <si>
+    <t>Child Care</t>
+  </si>
+  <si>
+    <t>Data Science</t>
   </si>
 </sst>
 </file>
@@ -805,7 +820,7 @@
     <col min="2" max="2" width="25.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +1212,7 @@
     <col min="2" max="2" width="35.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -1490,7 +1505,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1506,45 +1521,71 @@
       <c r="A1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>